<commit_message>
100 to 255 range data
</commit_message>
<xml_diff>
--- a/edited_data.xlsx
+++ b/edited_data.xlsx
@@ -1037,358 +1037,358 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C2" t="n">
-        <v>5</v>
+        <v>103</v>
       </c>
       <c r="D2" t="n">
-        <v>10</v>
+        <v>106</v>
       </c>
       <c r="E2" t="n">
-        <v>14</v>
+        <v>109</v>
       </c>
       <c r="F2" t="n">
-        <v>17</v>
+        <v>110</v>
       </c>
       <c r="G2" t="n">
-        <v>20</v>
+        <v>112</v>
       </c>
       <c r="H2" t="n">
-        <v>22</v>
+        <v>114</v>
       </c>
       <c r="I2" t="n">
-        <v>24</v>
+        <v>115</v>
       </c>
       <c r="J2" t="n">
-        <v>26</v>
+        <v>116</v>
       </c>
       <c r="K2" t="n">
-        <v>28</v>
+        <v>117</v>
       </c>
       <c r="L2" t="n">
-        <v>30</v>
+        <v>118</v>
       </c>
       <c r="M2" t="n">
-        <v>32</v>
+        <v>119</v>
       </c>
       <c r="N2" t="n">
-        <v>33</v>
+        <v>120</v>
       </c>
       <c r="O2" t="n">
-        <v>35</v>
+        <v>121</v>
       </c>
       <c r="P2" t="n">
-        <v>36</v>
+        <v>122</v>
       </c>
       <c r="Q2" t="n">
-        <v>37</v>
+        <v>123</v>
       </c>
       <c r="R2" t="n">
-        <v>39</v>
+        <v>124</v>
       </c>
       <c r="S2" t="n">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="T2" t="n">
-        <v>41</v>
+        <v>125</v>
       </c>
       <c r="U2" t="n">
-        <v>42</v>
+        <v>126</v>
       </c>
       <c r="V2" t="n">
-        <v>43</v>
+        <v>126</v>
       </c>
       <c r="W2" t="n">
-        <v>44</v>
+        <v>127</v>
       </c>
       <c r="X2" t="n">
-        <v>45</v>
+        <v>127</v>
       </c>
       <c r="Y2" t="n">
-        <v>45</v>
+        <v>128</v>
       </c>
       <c r="Z2" t="n">
-        <v>46</v>
+        <v>128</v>
       </c>
       <c r="AA2" t="n">
-        <v>47</v>
+        <v>129</v>
       </c>
       <c r="AB2" t="n">
-        <v>48</v>
+        <v>129</v>
       </c>
       <c r="AC2" t="n">
-        <v>49</v>
+        <v>130</v>
       </c>
       <c r="AD2" t="n">
-        <v>49</v>
+        <v>130</v>
       </c>
       <c r="AE2" t="n">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="AF2" t="n">
-        <v>51</v>
+        <v>131</v>
       </c>
       <c r="AG2" t="n">
-        <v>51</v>
+        <v>131</v>
       </c>
       <c r="AH2" t="n">
-        <v>52</v>
+        <v>131</v>
       </c>
       <c r="AI2" t="n">
-        <v>52</v>
+        <v>132</v>
       </c>
       <c r="AJ2" t="n">
-        <v>53</v>
+        <v>132</v>
       </c>
       <c r="AK2" t="n">
-        <v>54</v>
+        <v>133</v>
       </c>
       <c r="AL2" t="n">
-        <v>54</v>
+        <v>133</v>
       </c>
       <c r="AM2" t="n">
-        <v>55</v>
+        <v>133</v>
       </c>
       <c r="AN2" t="n">
-        <v>56</v>
+        <v>134</v>
       </c>
       <c r="AO2" t="n">
-        <v>56</v>
+        <v>134</v>
       </c>
       <c r="AP2" t="n">
-        <v>57</v>
+        <v>135</v>
       </c>
       <c r="AQ2" t="n">
-        <v>57</v>
+        <v>135</v>
       </c>
       <c r="AR2" t="n">
-        <v>58</v>
+        <v>135</v>
       </c>
       <c r="AS2" t="n">
-        <v>59</v>
+        <v>136</v>
       </c>
       <c r="AT2" t="n">
-        <v>59</v>
+        <v>136</v>
       </c>
       <c r="AU2" t="n">
-        <v>60</v>
+        <v>136</v>
       </c>
       <c r="AV2" t="n">
-        <v>60</v>
+        <v>137</v>
       </c>
       <c r="AW2" t="n">
-        <v>61</v>
+        <v>137</v>
       </c>
       <c r="AX2" t="n">
-        <v>61</v>
+        <v>137</v>
       </c>
       <c r="AY2" t="n">
-        <v>62</v>
+        <v>138</v>
       </c>
       <c r="AZ2" t="n">
-        <v>62</v>
+        <v>138</v>
       </c>
       <c r="BA2" t="n">
-        <v>63</v>
+        <v>138</v>
       </c>
       <c r="BB2" t="n">
-        <v>64</v>
+        <v>139</v>
       </c>
       <c r="BC2" t="n">
-        <v>65</v>
+        <v>139</v>
       </c>
       <c r="BD2" t="n">
-        <v>65</v>
+        <v>140</v>
       </c>
       <c r="BE2" t="n">
-        <v>66</v>
+        <v>140</v>
       </c>
       <c r="BF2" t="n">
-        <v>67</v>
+        <v>141</v>
       </c>
       <c r="BG2" t="n">
-        <v>67</v>
+        <v>141</v>
       </c>
       <c r="BH2" t="n">
-        <v>68</v>
+        <v>141</v>
       </c>
       <c r="BI2" t="n">
-        <v>69</v>
+        <v>142</v>
       </c>
       <c r="BJ2" t="n">
-        <v>70</v>
+        <v>142</v>
       </c>
       <c r="BK2" t="n">
-        <v>70</v>
+        <v>143</v>
       </c>
       <c r="BL2" t="n">
-        <v>71</v>
+        <v>143</v>
       </c>
       <c r="BM2" t="n">
-        <v>72</v>
+        <v>144</v>
       </c>
       <c r="BN2" t="n">
-        <v>72</v>
+        <v>144</v>
       </c>
       <c r="BO2" t="n">
-        <v>73</v>
+        <v>145</v>
       </c>
       <c r="BP2" t="n">
-        <v>74</v>
+        <v>145</v>
       </c>
       <c r="BQ2" t="n">
-        <v>75</v>
+        <v>145</v>
       </c>
       <c r="BR2" t="n">
-        <v>75</v>
+        <v>146</v>
       </c>
       <c r="BS2" t="n">
-        <v>76</v>
+        <v>146</v>
       </c>
       <c r="BT2" t="n">
-        <v>77</v>
+        <v>147</v>
       </c>
       <c r="BU2" t="n">
-        <v>78</v>
+        <v>147</v>
       </c>
       <c r="BV2" t="n">
-        <v>79</v>
+        <v>148</v>
       </c>
       <c r="BW2" t="n">
-        <v>79</v>
+        <v>148</v>
       </c>
       <c r="BX2" t="n">
-        <v>80</v>
+        <v>149</v>
       </c>
       <c r="BY2" t="n">
-        <v>81</v>
+        <v>149</v>
       </c>
       <c r="BZ2" t="n">
-        <v>81</v>
+        <v>149</v>
       </c>
       <c r="CA2" t="n">
-        <v>82</v>
+        <v>150</v>
       </c>
       <c r="CB2" t="n">
-        <v>82</v>
+        <v>150</v>
       </c>
       <c r="CC2" t="n">
-        <v>83</v>
+        <v>150</v>
       </c>
       <c r="CD2" t="n">
-        <v>83</v>
+        <v>151</v>
       </c>
       <c r="CE2" t="n">
-        <v>84</v>
+        <v>151</v>
       </c>
       <c r="CF2" t="n">
-        <v>84</v>
+        <v>151</v>
       </c>
       <c r="CG2" t="n">
-        <v>85</v>
+        <v>151</v>
       </c>
       <c r="CH2" t="n">
-        <v>85</v>
+        <v>152</v>
       </c>
       <c r="CI2" t="n">
-        <v>85</v>
+        <v>152</v>
       </c>
       <c r="CJ2" t="n">
-        <v>86</v>
+        <v>152</v>
       </c>
       <c r="CK2" t="n">
-        <v>86</v>
+        <v>152</v>
       </c>
       <c r="CL2" t="n">
-        <v>87</v>
+        <v>153</v>
       </c>
       <c r="CM2" t="n">
-        <v>87</v>
+        <v>153</v>
       </c>
       <c r="CN2" t="n">
-        <v>88</v>
+        <v>153</v>
       </c>
       <c r="CO2" t="n">
-        <v>88</v>
+        <v>154</v>
       </c>
       <c r="CP2" t="n">
-        <v>89</v>
+        <v>154</v>
       </c>
       <c r="CQ2" t="n">
-        <v>89</v>
+        <v>154</v>
       </c>
       <c r="CR2" t="n">
-        <v>90</v>
+        <v>154</v>
       </c>
       <c r="CS2" t="n">
-        <v>90</v>
+        <v>155</v>
       </c>
       <c r="CT2" t="n">
-        <v>91</v>
+        <v>155</v>
       </c>
       <c r="CU2" t="n">
-        <v>92</v>
+        <v>156</v>
       </c>
       <c r="CV2" t="n">
-        <v>92</v>
+        <v>156</v>
       </c>
       <c r="CW2" t="n">
-        <v>93</v>
+        <v>156</v>
       </c>
       <c r="CX2" t="n">
-        <v>94</v>
+        <v>157</v>
       </c>
       <c r="CY2" t="n">
-        <v>94</v>
+        <v>157</v>
       </c>
       <c r="CZ2" t="n">
-        <v>95</v>
+        <v>158</v>
       </c>
       <c r="DA2" t="n">
-        <v>95</v>
+        <v>158</v>
       </c>
       <c r="DB2" t="n">
-        <v>96</v>
+        <v>158</v>
       </c>
       <c r="DC2" t="n">
-        <v>96</v>
+        <v>159</v>
       </c>
       <c r="DD2" t="n">
-        <v>97</v>
+        <v>159</v>
       </c>
       <c r="DE2" t="n">
-        <v>98</v>
+        <v>159</v>
       </c>
       <c r="DF2" t="n">
-        <v>98</v>
+        <v>160</v>
       </c>
       <c r="DG2" t="n">
-        <v>99</v>
+        <v>160</v>
       </c>
       <c r="DH2" t="n">
-        <v>99</v>
+        <v>160</v>
       </c>
       <c r="DI2" t="n">
-        <v>100</v>
+        <v>161</v>
       </c>
       <c r="DJ2" t="n">
-        <v>100</v>
+        <v>161</v>
       </c>
       <c r="DK2" t="n">
-        <v>101</v>
+        <v>161</v>
       </c>
       <c r="DL2" t="n">
-        <v>101</v>
+        <v>162</v>
       </c>
       <c r="DM2" t="n">
-        <v>102</v>
+        <v>162</v>
       </c>
       <c r="DN2" t="n">
-        <v>103</v>
+        <v>162</v>
       </c>
       <c r="DO2" t="n">
-        <v>103</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3">
@@ -1398,358 +1398,358 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>72</v>
+        <v>144</v>
       </c>
       <c r="C3" t="n">
-        <v>73</v>
+        <v>144</v>
       </c>
       <c r="D3" t="n">
-        <v>74</v>
+        <v>145</v>
       </c>
       <c r="E3" t="n">
-        <v>74</v>
+        <v>145</v>
       </c>
       <c r="F3" t="n">
-        <v>75</v>
+        <v>145</v>
       </c>
       <c r="G3" t="n">
-        <v>75</v>
+        <v>146</v>
       </c>
       <c r="H3" t="n">
-        <v>76</v>
+        <v>146</v>
       </c>
       <c r="I3" t="n">
-        <v>76</v>
+        <v>146</v>
       </c>
       <c r="J3" t="n">
-        <v>77</v>
+        <v>147</v>
       </c>
       <c r="K3" t="n">
-        <v>78</v>
+        <v>147</v>
       </c>
       <c r="L3" t="n">
-        <v>78</v>
+        <v>148</v>
       </c>
       <c r="M3" t="n">
-        <v>79</v>
+        <v>148</v>
       </c>
       <c r="N3" t="n">
-        <v>80</v>
+        <v>148</v>
       </c>
       <c r="O3" t="n">
-        <v>80</v>
+        <v>149</v>
       </c>
       <c r="P3" t="n">
-        <v>81</v>
+        <v>149</v>
       </c>
       <c r="Q3" t="n">
-        <v>81</v>
+        <v>150</v>
       </c>
       <c r="R3" t="n">
-        <v>82</v>
+        <v>150</v>
       </c>
       <c r="S3" t="n">
-        <v>82</v>
+        <v>150</v>
       </c>
       <c r="T3" t="n">
-        <v>83</v>
+        <v>150</v>
       </c>
       <c r="U3" t="n">
-        <v>83</v>
+        <v>150</v>
       </c>
       <c r="V3" t="n">
-        <v>83</v>
+        <v>151</v>
       </c>
       <c r="W3" t="n">
-        <v>84</v>
+        <v>151</v>
       </c>
       <c r="X3" t="n">
-        <v>84</v>
+        <v>151</v>
       </c>
       <c r="Y3" t="n">
-        <v>85</v>
+        <v>152</v>
       </c>
       <c r="Z3" t="n">
-        <v>86</v>
+        <v>152</v>
       </c>
       <c r="AA3" t="n">
-        <v>86</v>
+        <v>152</v>
       </c>
       <c r="AB3" t="n">
-        <v>87</v>
+        <v>153</v>
       </c>
       <c r="AC3" t="n">
-        <v>87</v>
+        <v>153</v>
       </c>
       <c r="AD3" t="n">
-        <v>88</v>
+        <v>153</v>
       </c>
       <c r="AE3" t="n">
-        <v>89</v>
+        <v>154</v>
       </c>
       <c r="AF3" t="n">
-        <v>89</v>
+        <v>154</v>
       </c>
       <c r="AG3" t="n">
-        <v>90</v>
+        <v>155</v>
       </c>
       <c r="AH3" t="n">
-        <v>90</v>
+        <v>155</v>
       </c>
       <c r="AI3" t="n">
-        <v>91</v>
+        <v>155</v>
       </c>
       <c r="AJ3" t="n">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="AK3" t="n">
-        <v>92</v>
+        <v>156</v>
       </c>
       <c r="AL3" t="n">
-        <v>92</v>
+        <v>156</v>
       </c>
       <c r="AM3" t="n">
-        <v>93</v>
+        <v>156</v>
       </c>
       <c r="AN3" t="n">
-        <v>93</v>
+        <v>157</v>
       </c>
       <c r="AO3" t="n">
-        <v>94</v>
+        <v>157</v>
       </c>
       <c r="AP3" t="n">
-        <v>94</v>
+        <v>157</v>
       </c>
       <c r="AQ3" t="n">
-        <v>94</v>
+        <v>157</v>
       </c>
       <c r="AR3" t="n">
-        <v>95</v>
+        <v>158</v>
       </c>
       <c r="AS3" t="n">
-        <v>95</v>
+        <v>158</v>
       </c>
       <c r="AT3" t="n">
-        <v>95</v>
+        <v>158</v>
       </c>
       <c r="AU3" t="n">
-        <v>95</v>
+        <v>158</v>
       </c>
       <c r="AV3" t="n">
-        <v>96</v>
+        <v>158</v>
       </c>
       <c r="AW3" t="n">
-        <v>96</v>
+        <v>158</v>
       </c>
       <c r="AX3" t="n">
-        <v>97</v>
+        <v>159</v>
       </c>
       <c r="AY3" t="n">
-        <v>97</v>
+        <v>159</v>
       </c>
       <c r="AZ3" t="n">
-        <v>98</v>
+        <v>159</v>
       </c>
       <c r="BA3" t="n">
-        <v>98</v>
+        <v>160</v>
       </c>
       <c r="BB3" t="n">
-        <v>98</v>
+        <v>160</v>
       </c>
       <c r="BC3" t="n">
-        <v>99</v>
+        <v>160</v>
       </c>
       <c r="BD3" t="n">
-        <v>99</v>
+        <v>160</v>
       </c>
       <c r="BE3" t="n">
-        <v>100</v>
+        <v>161</v>
       </c>
       <c r="BF3" t="n">
-        <v>100</v>
+        <v>161</v>
       </c>
       <c r="BG3" t="n">
-        <v>101</v>
+        <v>161</v>
       </c>
       <c r="BH3" t="n">
-        <v>101</v>
+        <v>161</v>
       </c>
       <c r="BI3" t="n">
-        <v>102</v>
+        <v>162</v>
       </c>
       <c r="BJ3" t="n">
-        <v>102</v>
+        <v>162</v>
       </c>
       <c r="BK3" t="n">
-        <v>103</v>
+        <v>162</v>
       </c>
       <c r="BL3" t="n">
-        <v>103</v>
+        <v>163</v>
       </c>
       <c r="BM3" t="n">
-        <v>104</v>
+        <v>163</v>
       </c>
       <c r="BN3" t="n">
-        <v>104</v>
+        <v>163</v>
       </c>
       <c r="BO3" t="n">
-        <v>105</v>
+        <v>164</v>
       </c>
       <c r="BP3" t="n">
-        <v>105</v>
+        <v>164</v>
       </c>
       <c r="BQ3" t="n">
-        <v>106</v>
+        <v>164</v>
       </c>
       <c r="BR3" t="n">
-        <v>106</v>
+        <v>165</v>
       </c>
       <c r="BS3" t="n">
-        <v>107</v>
+        <v>165</v>
       </c>
       <c r="BT3" t="n">
-        <v>107</v>
+        <v>165</v>
       </c>
       <c r="BU3" t="n">
-        <v>108</v>
+        <v>166</v>
       </c>
       <c r="BV3" t="n">
-        <v>109</v>
+        <v>166</v>
       </c>
       <c r="BW3" t="n">
-        <v>109</v>
+        <v>167</v>
       </c>
       <c r="BX3" t="n">
-        <v>110</v>
+        <v>167</v>
       </c>
       <c r="BY3" t="n">
-        <v>111</v>
+        <v>167</v>
       </c>
       <c r="BZ3" t="n">
-        <v>111</v>
+        <v>168</v>
       </c>
       <c r="CA3" t="n">
-        <v>112</v>
+        <v>168</v>
       </c>
       <c r="CB3" t="n">
-        <v>112</v>
+        <v>168</v>
       </c>
       <c r="CC3" t="n">
-        <v>113</v>
+        <v>169</v>
       </c>
       <c r="CD3" t="n">
-        <v>114</v>
+        <v>169</v>
       </c>
       <c r="CE3" t="n">
-        <v>114</v>
+        <v>169</v>
       </c>
       <c r="CF3" t="n">
-        <v>114</v>
+        <v>170</v>
       </c>
       <c r="CG3" t="n">
-        <v>115</v>
+        <v>170</v>
       </c>
       <c r="CH3" t="n">
-        <v>115</v>
+        <v>170</v>
       </c>
       <c r="CI3" t="n">
-        <v>116</v>
+        <v>170</v>
       </c>
       <c r="CJ3" t="n">
-        <v>116</v>
+        <v>171</v>
       </c>
       <c r="CK3" t="n">
-        <v>116</v>
+        <v>171</v>
       </c>
       <c r="CL3" t="n">
-        <v>117</v>
+        <v>171</v>
       </c>
       <c r="CM3" t="n">
-        <v>117</v>
+        <v>171</v>
       </c>
       <c r="CN3" t="n">
-        <v>118</v>
+        <v>171</v>
       </c>
       <c r="CO3" t="n">
-        <v>118</v>
+        <v>172</v>
       </c>
       <c r="CP3" t="n">
-        <v>118</v>
+        <v>172</v>
       </c>
       <c r="CQ3" t="n">
-        <v>119</v>
+        <v>172</v>
       </c>
       <c r="CR3" t="n">
-        <v>119</v>
+        <v>172</v>
       </c>
       <c r="CS3" t="n">
-        <v>119</v>
+        <v>173</v>
       </c>
       <c r="CT3" t="n">
-        <v>120</v>
+        <v>173</v>
       </c>
       <c r="CU3" t="n">
-        <v>120</v>
+        <v>173</v>
       </c>
       <c r="CV3" t="n">
-        <v>121</v>
+        <v>173</v>
       </c>
       <c r="CW3" t="n">
-        <v>121</v>
+        <v>173</v>
       </c>
       <c r="CX3" t="n">
-        <v>121</v>
+        <v>174</v>
       </c>
       <c r="CY3" t="n">
-        <v>122</v>
+        <v>174</v>
       </c>
       <c r="CZ3" t="n">
-        <v>122</v>
+        <v>174</v>
       </c>
       <c r="DA3" t="n">
-        <v>122</v>
+        <v>174</v>
       </c>
       <c r="DB3" t="n">
-        <v>122</v>
+        <v>174</v>
       </c>
       <c r="DC3" t="n">
-        <v>123</v>
+        <v>175</v>
       </c>
       <c r="DD3" t="n">
-        <v>123</v>
+        <v>175</v>
       </c>
       <c r="DE3" t="n">
-        <v>123</v>
+        <v>175</v>
       </c>
       <c r="DF3" t="n">
-        <v>124</v>
+        <v>175</v>
       </c>
       <c r="DG3" t="n">
-        <v>124</v>
+        <v>175</v>
       </c>
       <c r="DH3" t="n">
-        <v>124</v>
+        <v>176</v>
       </c>
       <c r="DI3" t="n">
-        <v>124</v>
+        <v>176</v>
       </c>
       <c r="DJ3" t="n">
-        <v>125</v>
+        <v>176</v>
       </c>
       <c r="DK3" t="n">
-        <v>125</v>
+        <v>176</v>
       </c>
       <c r="DL3" t="n">
-        <v>125</v>
+        <v>176</v>
       </c>
       <c r="DM3" t="n">
-        <v>125</v>
+        <v>176</v>
       </c>
       <c r="DN3" t="n">
-        <v>126</v>
+        <v>176</v>
       </c>
       <c r="DO3" t="n">
-        <v>126</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4">
@@ -1759,337 +1759,337 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>125</v>
+        <v>176</v>
       </c>
       <c r="C4" t="n">
-        <v>126</v>
+        <v>177</v>
       </c>
       <c r="D4" t="n">
-        <v>127</v>
+        <v>177</v>
       </c>
       <c r="E4" t="n">
-        <v>128</v>
+        <v>178</v>
       </c>
       <c r="F4" t="n">
-        <v>129</v>
+        <v>179</v>
       </c>
       <c r="G4" t="n">
-        <v>130</v>
+        <v>179</v>
       </c>
       <c r="H4" t="n">
-        <v>131</v>
+        <v>180</v>
       </c>
       <c r="I4" t="n">
-        <v>132</v>
+        <v>181</v>
       </c>
       <c r="J4" t="n">
-        <v>133</v>
+        <v>181</v>
       </c>
       <c r="K4" t="n">
-        <v>134</v>
+        <v>182</v>
       </c>
       <c r="L4" t="n">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="M4" t="n">
-        <v>136</v>
+        <v>183</v>
       </c>
       <c r="N4" t="n">
-        <v>137</v>
+        <v>183</v>
       </c>
       <c r="O4" t="n">
-        <v>138</v>
+        <v>184</v>
       </c>
       <c r="P4" t="n">
-        <v>139</v>
+        <v>185</v>
       </c>
       <c r="Q4" t="n">
-        <v>140</v>
+        <v>185</v>
       </c>
       <c r="R4" t="n">
-        <v>141</v>
+        <v>186</v>
       </c>
       <c r="S4" t="n">
-        <v>142</v>
+        <v>186</v>
       </c>
       <c r="T4" t="n">
-        <v>142</v>
+        <v>187</v>
       </c>
       <c r="U4" t="n">
-        <v>143</v>
+        <v>187</v>
       </c>
       <c r="V4" t="n">
-        <v>144</v>
+        <v>188</v>
       </c>
       <c r="W4" t="n">
-        <v>145</v>
+        <v>188</v>
       </c>
       <c r="X4" t="n">
-        <v>145</v>
+        <v>188</v>
       </c>
       <c r="Y4" t="n">
-        <v>146</v>
+        <v>189</v>
       </c>
       <c r="Z4" t="n">
-        <v>147</v>
+        <v>189</v>
       </c>
       <c r="AA4" t="n">
-        <v>147</v>
+        <v>190</v>
       </c>
       <c r="AB4" t="n">
-        <v>148</v>
+        <v>190</v>
       </c>
       <c r="AC4" t="n">
-        <v>149</v>
+        <v>190</v>
       </c>
       <c r="AD4" t="n">
-        <v>149</v>
+        <v>191</v>
       </c>
       <c r="AE4" t="n">
-        <v>150</v>
+        <v>191</v>
       </c>
       <c r="AF4" t="n">
-        <v>150</v>
+        <v>191</v>
       </c>
       <c r="AG4" t="n">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="AH4" t="n">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="AI4" t="n">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="AJ4" t="n">
-        <v>152</v>
+        <v>192</v>
       </c>
       <c r="AK4" t="n">
-        <v>152</v>
+        <v>193</v>
       </c>
       <c r="AL4" t="n">
-        <v>153</v>
+        <v>193</v>
       </c>
       <c r="AM4" t="n">
-        <v>153</v>
+        <v>193</v>
       </c>
       <c r="AN4" t="n">
-        <v>154</v>
+        <v>193</v>
       </c>
       <c r="AO4" t="n">
-        <v>154</v>
+        <v>194</v>
       </c>
       <c r="AP4" t="n">
-        <v>154</v>
+        <v>194</v>
       </c>
       <c r="AQ4" t="n">
-        <v>155</v>
+        <v>194</v>
       </c>
       <c r="AR4" t="n">
-        <v>155</v>
+        <v>194</v>
       </c>
       <c r="AS4" t="n">
-        <v>156</v>
+        <v>195</v>
       </c>
       <c r="AT4" t="n">
-        <v>156</v>
+        <v>195</v>
       </c>
       <c r="AU4" t="n">
-        <v>157</v>
+        <v>195</v>
       </c>
       <c r="AV4" t="n">
-        <v>157</v>
+        <v>196</v>
       </c>
       <c r="AW4" t="n">
-        <v>158</v>
+        <v>196</v>
       </c>
       <c r="AX4" t="n">
-        <v>158</v>
+        <v>196</v>
       </c>
       <c r="AY4" t="n">
-        <v>159</v>
+        <v>196</v>
       </c>
       <c r="AZ4" t="n">
-        <v>159</v>
+        <v>197</v>
       </c>
       <c r="BA4" t="n">
-        <v>159</v>
+        <v>197</v>
       </c>
       <c r="BB4" t="n">
-        <v>160</v>
+        <v>197</v>
       </c>
       <c r="BC4" t="n">
-        <v>160</v>
+        <v>197</v>
       </c>
       <c r="BD4" t="n">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="BE4" t="n">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="BF4" t="n">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="BG4" t="n">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="BH4" t="n">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="BI4" t="n">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="BJ4" t="n">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BK4" t="n">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="BL4" t="n">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="BM4" t="n">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="BN4" t="n">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="BO4" t="n">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="BP4" t="n">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="BQ4" t="n">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="BR4" t="n">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="BS4" t="n">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="BT4" t="n">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="BU4" t="n">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="BV4" t="n">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="BW4" t="n">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="BX4" t="n">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="BY4" t="n">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="BZ4" t="n">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="CA4" t="n">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="CB4" t="n">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="CC4" t="n">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="CD4" t="n">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="CE4" t="n">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="CF4" t="n">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="CG4" t="n">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="CH4" t="n">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="CI4" t="n">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="CJ4" t="n">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="CK4" t="n">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="CL4" t="n">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="CM4" t="n">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="CN4" t="n">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="CO4" t="n">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="CP4" t="n">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="CQ4" t="n">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="CR4" t="n">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="CS4" t="n">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="CT4" t="n">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="CU4" t="n">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="CV4" t="n">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="CW4" t="n">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="CX4" t="n">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="CY4" t="n">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="CZ4" t="n">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="DA4" t="n">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="DB4" t="n">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="DC4" t="n">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="DD4" t="n">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="DE4" t="n">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="DF4" t="n">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="DG4" t="n">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="DH4" t="n">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="DI4" t="n">
         <v>254</v>
@@ -2101,7 +2101,7 @@
         <v>254</v>
       </c>
       <c r="DL4" t="n">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="DM4" t="n">
         <v>255</v>

</xml_diff>